<commit_message>
Add rubric format heuristics to translation prompt
Translation prompt now includes parsing rules for:
- Comma-separated hierarchy (general → specific)
- "of" suffix referring back to parent rubric
- Abbreviations (agg., amel.)
- Time/condition modifiers
- Subrubric context inheritance

Cost increase ~10% ($28→$31 for full repertory) - worth it for accuracy.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/tests/translation_cost_comparison.xlsx
+++ b/tests/translation_cost_comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Details" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Details" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,97 +478,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>269.4</v>
+        <v>445.6</v>
       </c>
       <c r="C2" t="n">
-        <v>190</v>
+        <v>241.1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000305</v>
+        <v>0.000413</v>
       </c>
       <c r="E2" t="n">
-        <v>1.8</v>
+        <v>2.44</v>
       </c>
       <c r="F2" t="n">
-        <v>22.74</v>
+        <v>30.79</v>
       </c>
       <c r="G2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>claude-sonnet-4-20250514</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>269.4</v>
-      </c>
-      <c r="C3" t="n">
-        <v>187.2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.003616</v>
-      </c>
-      <c r="E3" t="n">
-        <v>21.34</v>
-      </c>
-      <c r="F3" t="n">
-        <v>269.77</v>
-      </c>
-      <c r="G3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>gpt-4o-mini</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>245.6</v>
-      </c>
-      <c r="C4" t="n">
-        <v>179.2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.000144</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="F4" t="n">
-        <v>10.77</v>
-      </c>
-      <c r="G4" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>gpt-4o</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>245.6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>170.4</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.002318</v>
-      </c>
-      <c r="E5" t="n">
-        <v>13.68</v>
-      </c>
-      <c r="F5" t="n">
-        <v>172.92</v>
-      </c>
-      <c r="G5" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -582,7 +507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -643,113 +568,113 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Delusions of being in eternity or immortality</t>
+          <t>Delusion of being in eternity</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>270</v>
+        <v>445</v>
       </c>
       <c r="F2" t="n">
-        <v>183</v>
+        <v>263</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00029625</v>
+        <v>0.00044</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>47040</v>
+        <v>46193</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mind, delusions, eternity, that he was in</t>
+          <t>Mind, anxiety, forenoon</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>claude-sonnet-4-20250514</t>
+          <t>claude-3-haiku-20240307</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>belief that one exists in eternity or outside of time</t>
+          <t>Anxiety experienced in the late morning/forenoon</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>270</v>
+        <v>440</v>
       </c>
       <c r="F3" t="n">
-        <v>169</v>
+        <v>211</v>
       </c>
       <c r="G3" t="n">
-        <v>0.003345</v>
+        <v>0.00037375</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>47040</v>
+        <v>49200</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mind, delusions, eternity, that he was in</t>
+          <t>Mind, restlessness, menses, during</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>gpt-4o-mini</t>
+          <t>claude-3-haiku-20240307</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>a belief that one is experiencing eternal existence</t>
+          <t>Restlessness during menstruation</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>246</v>
+        <v>443</v>
       </c>
       <c r="F4" t="n">
-        <v>172</v>
+        <v>241</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0001401</v>
+        <v>0.000412</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>47040</v>
+        <v>48718</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mind, delusions, eternity, that he was in</t>
+          <t>Mind, kleptomania, steals money</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-haiku-20240307</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Belief of being trapped in time without end</t>
+          <t>Compulsive urge to steal money</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>246</v>
+        <v>443</v>
       </c>
       <c r="F5" t="n">
-        <v>185</v>
+        <v>234</v>
       </c>
       <c r="G5" t="n">
-        <v>0.002465</v>
+        <v>0.00040325</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>46193</v>
+        <v>49192</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mind, anxiety, forenoon</t>
+          <t>Mind, restlessness, internal, as if would beat about herself with hands and feet</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -759,113 +684,113 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Anxiety in the morning</t>
+          <t>An inner restlessness and urge to move the hands and feet aggressively</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>265</v>
+        <v>451</v>
       </c>
       <c r="F6" t="n">
-        <v>175</v>
+        <v>245</v>
       </c>
       <c r="G6" t="n">
-        <v>0.000285</v>
+        <v>0.000419</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>46193</v>
+        <v>103886</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mind, anxiety, forenoon</t>
+          <t>Mind, mistakes, writing</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>claude-sonnet-4-20250514</t>
+          <t>claude-3-haiku-20240307</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Anxiety occurring specifically during the morning hours before noon</t>
+          <t>Difficulty concentrating when writing, tendency to make mistakes in writing</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>265</v>
+        <v>438</v>
       </c>
       <c r="F7" t="n">
-        <v>160</v>
+        <v>282</v>
       </c>
       <c r="G7" t="n">
-        <v>0.003195</v>
+        <v>0.000462</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>46193</v>
+        <v>49181</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mind, anxiety, forenoon</t>
+          <t>Mind, restlessness, evening, 6 p.m. till 6 a.m.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>gpt-4o-mini</t>
+          <t>claude-3-haiku-20240307</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Anxiety during the morning hours.</t>
+          <t>Restlessness in the evenings from 6 PM to 6 AM</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>242</v>
+        <v>456</v>
       </c>
       <c r="F8" t="n">
-        <v>147</v>
+        <v>209</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0001245</v>
+        <v>0.00037525</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>46193</v>
+        <v>47216</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mind, anxiety, forenoon</t>
+          <t>Mind, delusions, inkstand, fancied he saw one on bed</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>claude-3-haiku-20240307</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>anxiety in the late morning</t>
+          <t>A false belief that there is an inkstand on the bed</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>242</v>
+        <v>449</v>
       </c>
       <c r="F9" t="n">
-        <v>148</v>
+        <v>241</v>
       </c>
       <c r="G9" t="n">
-        <v>0.002085</v>
+        <v>0.0004135</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>49200</v>
+        <v>47467</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mind, restlessness, menses, during</t>
+          <t>Mind, delusions, spectres, pursued by, is</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -875,336 +800,46 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Restlessness during menstruation</t>
+          <t>A feeling of being pursued by spectres or phantoms</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>268</v>
+        <v>445</v>
       </c>
       <c r="F10" t="n">
-        <v>191</v>
+        <v>253</v>
       </c>
       <c r="G10" t="n">
-        <v>0.00030575</v>
+        <v>0.0004275</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>49200</v>
+        <v>103783</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Mind, restlessness, menses, during</t>
+          <t>Mind, delusions, images, phantoms, closing the eyes</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>claude-sonnet-4-20250514</t>
+          <t>claude-3-haiku-20240307</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>restlessness during menstrual periods</t>
+          <t>Seeing phantom images or hallucinations when eyes are closed</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>268</v>
+        <v>446</v>
       </c>
       <c r="F11" t="n">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="G11" t="n">
-        <v>0.003744</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>49200</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Mind, restlessness, menses, during</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>gpt-4o-mini</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>restlessness during menstruation</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>244</v>
-      </c>
-      <c r="F12" t="n">
-        <v>182</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.0001458</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>49200</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Mind, restlessness, menses, during</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>gpt-4o</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>increased restlessness during menstruation</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>244</v>
-      </c>
-      <c r="F13" t="n">
-        <v>172</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.00233</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>48718</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Mind, kleptomania, steals money</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>claude-3-haiku-20240307</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>a tendency to steal money</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>268</v>
-      </c>
-      <c r="F14" t="n">
-        <v>194</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.0003095</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>48718</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Mind, kleptomania, steals money</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>claude-sonnet-4-20250514</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Compulsive stealing of money</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>268</v>
-      </c>
-      <c r="F15" t="n">
-        <v>195</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.003729</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>48718</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Mind, kleptomania, steals money</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>gpt-4o-mini</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>compulsive stealing of money</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>244</v>
-      </c>
-      <c r="F16" t="n">
-        <v>186</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.0001482</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>48718</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Mind, kleptomania, steals money</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>gpt-4o</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>a compulsion to steal money</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>244</v>
-      </c>
-      <c r="F17" t="n">
-        <v>179</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.0024</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>49192</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Mind, restlessness, internal, as if would beat about herself with hands and feet</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>claude-3-haiku-20240307</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Restlessness, with an urge to move hands and feet.</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>276</v>
-      </c>
-      <c r="F18" t="n">
-        <v>207</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.00032775</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>49192</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Mind, restlessness, internal, as if would beat about herself with hands and feet</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>claude-sonnet-4-20250514</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Internal restlessness with urge to flail arms and legs wildly</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>276</v>
-      </c>
-      <c r="F19" t="n">
-        <v>216</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.004068</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>49192</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Mind, restlessness, internal, as if would beat about herself with hands and feet</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>gpt-4o-mini</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>an internal sense of restlessness as if wanting to thrash around</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
-        <v>252</v>
-      </c>
-      <c r="F20" t="n">
-        <v>209</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.0001632</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>49192</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Mind, restlessness, internal, as if would beat about herself with hands and feet</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>gpt-4o</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>intense inner agitation and fidgeting</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>252</v>
-      </c>
-      <c r="F21" t="n">
-        <v>168</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.00231</v>
+        <v>0.0004015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve translation prompt heuristics and add LLM judge
Fixed ~9% error rate in translations by adding critical pattern rules:
- "ailments after X" = symptoms caused by X (not tendency)
- "speech, answers" = specifically about answering questions
- Archaic word order warnings
- ", after" suffix = what happens after preceding event

Added scripts/judge_translations.py to score translations on
detail preservation, accuracy, and clarity (1-5 scale each).

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/tests/translation_cost_comparison.xlsx
+++ b/tests/translation_cost_comparison.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,22 +478,97 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>445.6</v>
+        <v>444.4</v>
       </c>
       <c r="C2" t="n">
-        <v>241.1</v>
+        <v>234</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000413</v>
+        <v>0.000404</v>
       </c>
       <c r="E2" t="n">
-        <v>2.44</v>
+        <v>2.38</v>
       </c>
       <c r="F2" t="n">
-        <v>30.79</v>
+        <v>30.11</v>
       </c>
       <c r="G2" t="n">
-        <v>10</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>claude-sonnet-4-20250514</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>444.4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>244</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.004993</v>
+      </c>
+      <c r="E3" t="n">
+        <v>29.46</v>
+      </c>
+      <c r="F3" t="n">
+        <v>372.49</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>gpt-4o-mini</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>406.6</v>
+      </c>
+      <c r="C4" t="n">
+        <v>192.6</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.000177</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="F4" t="n">
+        <v>13.17</v>
+      </c>
+      <c r="G4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>406.6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>189.6</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.002912</v>
+      </c>
+      <c r="E5" t="n">
+        <v>17.18</v>
+      </c>
+      <c r="F5" t="n">
+        <v>217.27</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -507,7 +582,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,113 +643,113 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Delusion of being in eternity</t>
+          <t>a delusional belief that one is in eternity</t>
         </is>
       </c>
       <c r="E2" t="n">
         <v>445</v>
       </c>
       <c r="F2" t="n">
-        <v>263</v>
+        <v>231</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00044</v>
+        <v>0.0004</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>46193</v>
+        <v>47040</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mind, anxiety, forenoon</t>
+          <t>Mind, delusions, eternity, that he was in</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>claude-3-haiku-20240307</t>
+          <t>claude-sonnet-4-20250514</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Anxiety experienced in the late morning/forenoon</t>
+          <t>delusion of being in eternity</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="F3" t="n">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="G3" t="n">
-        <v>0.00037375</v>
+        <v>0.00486</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>49200</v>
+        <v>47040</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mind, restlessness, menses, during</t>
+          <t>Mind, delusions, eternity, that he was in</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>claude-3-haiku-20240307</t>
+          <t>gpt-4o-mini</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Restlessness during menstruation</t>
+          <t>delusion of being in eternity</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>443</v>
+        <v>407</v>
       </c>
       <c r="F4" t="n">
-        <v>241</v>
+        <v>187</v>
       </c>
       <c r="G4" t="n">
-        <v>0.000412</v>
+        <v>0.00017325</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>48718</v>
+        <v>47040</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mind, kleptomania, steals money</t>
+          <t>Mind, delusions, eternity, that he was in</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>claude-3-haiku-20240307</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Compulsive urge to steal money</t>
+          <t>belief of being in eternity</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>443</v>
+        <v>407</v>
       </c>
       <c r="F5" t="n">
-        <v>234</v>
+        <v>167</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00040325</v>
+        <v>0.0026875</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>49192</v>
+        <v>46193</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mind, restlessness, internal, as if would beat about herself with hands and feet</t>
+          <t>Mind, anxiety, forenoon</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -684,113 +759,113 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>An inner restlessness and urge to move the hands and feet aggressively</t>
+          <t>Tendency to experience anxiety during the forenoon</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="F6" t="n">
-        <v>245</v>
+        <v>193</v>
       </c>
       <c r="G6" t="n">
-        <v>0.000419</v>
+        <v>0.00035125</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>103886</v>
+        <v>46193</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mind, mistakes, writing</t>
+          <t>Mind, anxiety, forenoon</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>claude-3-haiku-20240307</t>
+          <t>claude-sonnet-4-20250514</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Difficulty concentrating when writing, tendency to make mistakes in writing</t>
+          <t>anxiety occurring in the forenoon (late morning hours)</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="F7" t="n">
-        <v>282</v>
+        <v>221</v>
       </c>
       <c r="G7" t="n">
-        <v>0.000462</v>
+        <v>0.004635</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>49181</v>
+        <v>46193</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mind, restlessness, evening, 6 p.m. till 6 a.m.</t>
+          <t>Mind, anxiety, forenoon</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>claude-3-haiku-20240307</t>
+          <t>gpt-4o-mini</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Restlessness in the evenings from 6 PM to 6 AM</t>
+          <t>anxiety in the forenoon</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>456</v>
+        <v>403</v>
       </c>
       <c r="F8" t="n">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00037525</v>
+        <v>0.00016785</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>47216</v>
+        <v>46193</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mind, delusions, inkstand, fancied he saw one on bed</t>
+          <t>Mind, anxiety, forenoon</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>claude-3-haiku-20240307</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>A false belief that there is an inkstand on the bed</t>
+          <t>anxiety in the late morning</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>449</v>
+        <v>403</v>
       </c>
       <c r="F9" t="n">
-        <v>241</v>
+        <v>183</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0004135</v>
+        <v>0.0028375</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>47467</v>
+        <v>49200</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mind, delusions, spectres, pursued by, is</t>
+          <t>Mind, restlessness, menses, during</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -800,46 +875,336 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>A feeling of being pursued by spectres or phantoms</t>
+          <t>Restlessness during menstruation</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F10" t="n">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0004275</v>
+        <v>0.00043325</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>103783</v>
+        <v>49200</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Mind, delusions, images, phantoms, closing the eyes</t>
+          <t>Mind, restlessness, menses, during</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>claude-sonnet-4-20250514</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>restlessness during menstruation</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>443</v>
+      </c>
+      <c r="F11" t="n">
+        <v>288</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.005649</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>49200</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Mind, restlessness, menses, during</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>gpt-4o-mini</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>restlessness during menstruation</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>405</v>
+      </c>
+      <c r="F12" t="n">
+        <v>196</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.00017835</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>49200</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Mind, restlessness, menses, during</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>restlessness during menstruation</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>405</v>
+      </c>
+      <c r="F13" t="n">
+        <v>197</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0029825</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>48718</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Mind, kleptomania, steals money</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>claude-3-haiku-20240307</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Seeing phantom images or hallucinations when eyes are closed</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>446</v>
-      </c>
-      <c r="F11" t="n">
-        <v>232</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.0004015</v>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>a tendency to steal money</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>443</v>
+      </c>
+      <c r="F14" t="n">
+        <v>205</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.000367</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>48718</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Mind, kleptomania, steals money</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>claude-sonnet-4-20250514</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>compulsive stealing of money</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>443</v>
+      </c>
+      <c r="F15" t="n">
+        <v>212</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.004509</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>48718</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Mind, kleptomania, steals money</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>gpt-4o-mini</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>compulsive stealing of money</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>405</v>
+      </c>
+      <c r="F16" t="n">
+        <v>178</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.00016755</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>48718</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Mind, kleptomania, steals money</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>a compulsion to steal money</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>405</v>
+      </c>
+      <c r="F17" t="n">
+        <v>171</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.0027225</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>49192</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Mind, restlessness, internal, as if would beat about herself with hands and feet</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>claude-3-haiku-20240307</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Restless inner agitation, as if needing to physically move about</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>451</v>
+      </c>
+      <c r="F18" t="n">
+        <v>283</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.0004665</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>49192</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Mind, restlessness, internal, as if would beat about herself with hands and feet</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>claude-sonnet-4-20250514</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>internal restlessness with urge to thrash about with hands and feet</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>451</v>
+      </c>
+      <c r="F19" t="n">
+        <v>264</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.005313</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>49192</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Mind, restlessness, internal, as if would beat about herself with hands and feet</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>gpt-4o-mini</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>inner restlessness, feeling a need to thrash about with hands and feet</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>413</v>
+      </c>
+      <c r="F20" t="n">
+        <v>223</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.00019575</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>49192</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Mind, restlessness, internal, as if would beat about herself with hands and feet</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>feeling an internal restlessness that makes them want to thrash about</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>413</v>
+      </c>
+      <c r="F21" t="n">
+        <v>230</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.0033325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>